<commit_message>
names edited in diagrams and tables for consistency
</commit_message>
<xml_diff>
--- a/robot_path_costmap/benchmark_results/comparison.xlsx
+++ b/robot_path_costmap/benchmark_results/comparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni\Auswertung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni\DrivingSwarm\multi_robot_path_planning_new\robot_path_costmap\benchmark_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170A791C-9EF4-44FC-9D97-B4B563B099C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7477BE17-BAEC-41AF-8B5F-572585915158}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{488D60FA-2164-4BC1-B819-175F70996519}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{488D60FA-2164-4BC1-B819-175F70996519}"/>
   </bookViews>
   <sheets>
     <sheet name="comparison 4" sheetId="1" r:id="rId1"/>
@@ -93,25 +93,25 @@
     <t>Total waypoint time [min]</t>
   </si>
   <si>
-    <t>collvoid 2-rooms: 8</t>
-  </si>
-  <si>
     <t>8 robots</t>
   </si>
   <si>
     <t>4 robots</t>
   </si>
   <si>
-    <t>path_layer 2-rooms: 4</t>
-  </si>
-  <si>
     <t>dwa tb3-world: 5</t>
   </si>
   <si>
-    <t>path_layer tb3-world: 5</t>
+    <t>Path Costmap</t>
   </si>
   <si>
-    <t>Path Layer</t>
+    <t>path costmap 2-rooms: 8</t>
+  </si>
+  <si>
+    <t>path costmap 2-rooms: 4</t>
+  </si>
+  <si>
+    <t>path costmap tb3-world: 5</t>
   </si>
 </sst>
 </file>
@@ -448,6 +448,17 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -484,17 +495,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -718,7 +718,7 @@
                   <c:v>DWA Local Planner</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Path Layer</c:v>
+                  <c:v>Path Costmap</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1222,7 +1222,7 @@
                   <c:v>DWA Local Planner</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Path Layer</c:v>
+                  <c:v>Path Costmap</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1704,7 +1704,7 @@
                   <c:v>DWA Local Planner</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Path Layer</c:v>
+                  <c:v>Path Costmap</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2012,7 +2012,7 @@
                   <c:v>DWA Local Planner</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Path Layer</c:v>
+                  <c:v>Path Costmap</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2071,7 +2071,7 @@
                   <c:v>DWA Local Planner</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Path Layer</c:v>
+                  <c:v>Path Costmap</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2497,7 +2497,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Path Layer</c:v>
+                  <c:v>Path Costmap</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6074,8 +6074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF431962-CEAC-4B55-A6AE-3CFE946E6CA0}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6092,29 +6092,29 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="46" t="s">
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="45"/>
+      <c r="H2" s="56"/>
       <c r="J2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="44" t="s">
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="45"/>
+      <c r="P2" s="56"/>
     </row>
     <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="30" t="s">
@@ -6238,13 +6238,13 @@
       <c r="K5" s="15">
         <v>98.581111111111127</v>
       </c>
-      <c r="L5" s="55">
+      <c r="L5" s="43">
         <v>30.268888888888892</v>
       </c>
-      <c r="M5" s="55">
+      <c r="M5" s="43">
         <v>19.068888888888885</v>
       </c>
-      <c r="N5" s="56">
+      <c r="N5" s="44">
         <v>21.312222222222218</v>
       </c>
       <c r="O5" s="14">
@@ -6286,13 +6286,13 @@
       <c r="K6" s="15">
         <v>88.580714285714294</v>
       </c>
-      <c r="L6" s="55">
+      <c r="L6" s="43">
         <v>34.160000000000004</v>
       </c>
-      <c r="M6" s="55">
+      <c r="M6" s="43">
         <v>20.04</v>
       </c>
-      <c r="N6" s="56">
+      <c r="N6" s="44">
         <v>23.294615384615383</v>
       </c>
       <c r="O6" s="14">
@@ -6411,31 +6411,31 @@
     <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="49" t="s">
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="43"/>
+      <c r="H14" s="54"/>
       <c r="J14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="42" t="s">
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="P14" s="43"/>
+      <c r="P14" s="54"/>
     </row>
     <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="16" t="s">
@@ -6783,13 +6783,13 @@
         <v>17</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6846,8 +6846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6C3372-B536-4B9E-8853-82CF1F213029}">
   <dimension ref="A2:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6863,25 +6863,25 @@
         <v>16</v>
       </c>
       <c r="C3" s="36"/>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="51"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="62"/>
       <c r="H3" t="s">
         <v>10</v>
       </c>
       <c r="M3" s="37" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N3" s="36"/>
-      <c r="O3" s="50" t="s">
+      <c r="O3" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="51"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
+      <c r="R3" s="62"/>
       <c r="S3" t="s">
         <v>10</v>
       </c>
@@ -6929,7 +6929,7 @@
       </c>
     </row>
     <row r="5" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="63" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="16" t="s">
@@ -6955,7 +6955,7 @@
         <f t="shared" ref="I5:I13" si="1">H5/60</f>
         <v>15.550542517516666</v>
       </c>
-      <c r="M5" s="52" t="s">
+      <c r="M5" s="63" t="s">
         <v>9</v>
       </c>
       <c r="N5" s="16" t="s">
@@ -6983,7 +6983,7 @@
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="52"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="16" t="s">
         <v>5</v>
       </c>
@@ -7007,7 +7007,7 @@
         <f t="shared" si="1"/>
         <v>14.896105217914998</v>
       </c>
-      <c r="M6" s="52"/>
+      <c r="M6" s="63"/>
       <c r="N6" s="16" t="s">
         <v>5</v>
       </c>
@@ -7028,12 +7028,12 @@
         <v>649.68200000000013</v>
       </c>
       <c r="T6" s="35">
-        <f t="shared" ref="T6:T13" si="3">S6/60</f>
+        <f t="shared" ref="T6:T12" si="3">S6/60</f>
         <v>10.828033333333336</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="52"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="16" t="s">
         <v>4</v>
       </c>
@@ -7057,7 +7057,7 @@
         <f t="shared" si="1"/>
         <v>16.134230887880001</v>
       </c>
-      <c r="M7" s="52"/>
+      <c r="M7" s="63"/>
       <c r="N7" s="16" t="s">
         <v>4</v>
       </c>
@@ -7083,7 +7083,7 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="52"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="16" t="s">
         <v>3</v>
       </c>
@@ -7107,7 +7107,7 @@
         <f t="shared" si="1"/>
         <v>14.448092412949999</v>
       </c>
-      <c r="M8" s="52"/>
+      <c r="M8" s="63"/>
       <c r="N8" s="16" t="s">
         <v>3</v>
       </c>
@@ -7133,7 +7133,7 @@
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="52"/>
+      <c r="B9" s="63"/>
       <c r="C9" s="16" t="s">
         <v>2</v>
       </c>
@@ -7157,7 +7157,7 @@
         <f t="shared" si="1"/>
         <v>14.242083597200001</v>
       </c>
-      <c r="M9" s="52"/>
+      <c r="M9" s="63"/>
       <c r="N9" s="16" t="s">
         <v>2</v>
       </c>
@@ -7183,7 +7183,7 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="52"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="16" t="s">
         <v>14</v>
       </c>
@@ -7207,7 +7207,7 @@
         <f t="shared" si="1"/>
         <v>14.930221482111669</v>
       </c>
-      <c r="M10" s="52"/>
+      <c r="M10" s="63"/>
       <c r="N10" s="16" t="s">
         <v>14</v>
       </c>
@@ -7233,7 +7233,7 @@
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="52"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="16" t="s">
         <v>13</v>
       </c>
@@ -7257,7 +7257,7 @@
         <f t="shared" si="1"/>
         <v>15.893974848581667</v>
       </c>
-      <c r="M11" s="52"/>
+      <c r="M11" s="63"/>
       <c r="N11" s="16" t="s">
         <v>13</v>
       </c>
@@ -7283,7 +7283,7 @@
       </c>
     </row>
     <row r="12" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="52"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="16" t="s">
         <v>12</v>
       </c>
@@ -7307,7 +7307,7 @@
         <f t="shared" si="1"/>
         <v>13.24469791255</v>
       </c>
-      <c r="M12" s="53"/>
+      <c r="M12" s="64"/>
       <c r="N12" s="16" t="s">
         <v>12</v>
       </c>
@@ -7395,37 +7395,37 @@
       <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="58" t="s">
-        <v>25</v>
+      <c r="C18" s="46" t="s">
+        <v>22</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="57"/>
-      <c r="J18" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="45"/>
+      <c r="J18" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="52" t="s">
         <v>20</v>
-      </c>
-      <c r="K18" s="64" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="64" t="s">
+      <c r="A19" s="52" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2">
         <f>I13</f>
         <v>14.917493609588123</v>
       </c>
-      <c r="C19" s="61">
+      <c r="C19" s="49">
         <f>T13</f>
         <v>11.709617038690476</v>
       </c>
-      <c r="E19" s="59" t="s">
-        <v>21</v>
+      <c r="E19" s="47" t="s">
+        <v>20</v>
       </c>
       <c r="F19" s="2">
         <v>3.2515527553628787</v>
@@ -7433,10 +7433,10 @@
       <c r="G19" s="2">
         <v>4.790395408868636</v>
       </c>
-      <c r="I19" s="62" t="s">
+      <c r="I19" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="54">
+      <c r="J19" s="42">
         <f>I13</f>
         <v>14.917493609588123</v>
       </c>
@@ -7449,10 +7449,10 @@
       <c r="A20" s="40"/>
       <c r="B20" s="41"/>
       <c r="C20" s="41"/>
-      <c r="E20" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="63">
+      <c r="E20" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="51">
         <f>I13</f>
         <v>14.917493609588123</v>
       </c>
@@ -7460,10 +7460,10 @@
         <f>T13</f>
         <v>11.709617038690476</v>
       </c>
-      <c r="I20" s="58" t="s">
-        <v>25</v>
-      </c>
-      <c r="J20" s="61">
+      <c r="I20" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="49">
         <f>T13</f>
         <v>11.709617038690476</v>
       </c>

</xml_diff>